<commit_message>
feat: ui: show a block around edit section
</commit_message>
<xml_diff>
--- a/examples/test.xlsx
+++ b/examples/test.xlsx
@@ -60,7 +60,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -72,6 +72,9 @@
         <v>10</v>
       </c>
       <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: `x` in range mode will extend the range
</commit_message>
<xml_diff>
--- a/examples/test.xlsx
+++ b/examples/test.xlsx
@@ -60,7 +60,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -69,27 +69,21 @@
   <sheetData>
     <row r="1">
       <c r="A1">
-        <v>10</v>
+        <v>1</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>0</v>
+      <c r="B1">
+        <f>A1*2</f>
+        <v>2</v>
       </c>
     </row>
     <row r="2">
       <c r="A2">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>30</v>
-      </c>
-      <c r="B3">
-        <f>SUM(A1:A3)</f>
-        <v>50</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chore: update example sheet
</commit_message>
<xml_diff>
--- a/examples/test.xlsx
+++ b/examples/test.xlsx
@@ -22,6 +22,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="45" formatCode="dd/mm/yyyy"/>
+  </numFmts>
   <fonts count="1">
     <font>
       <sz val="11"/>
@@ -48,8 +51,9 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1" applyFill="1"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf xfId="0" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf xfId="0" borderId="0" fillId="0" fontId="0" numFmtId="45"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="normal" builtinId="0"/>
@@ -60,7 +64,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -86,6 +90,15 @@
         <v>3</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" s="1">
+        <f>DATE(2025,2,26)</f>
+        <v>45714</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6"/>
+    </row>
   </sheetData>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
wip: different keybinds for bold and italic
</commit_message>
<xml_diff>
--- a/examples/test.xlsx
+++ b/examples/test.xlsx
@@ -13,9 +13,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t/>
+  </si>
+  <si>
+    <t>I am bold</t>
+  </si>
+  <si>
+    <t>I am italic</t>
+  </si>
+  <si>
+    <t>I am both</t>
+  </si>
+  <si>
+    <t>I am plain</t>
   </si>
 </sst>
 </file>
@@ -25,11 +37,36 @@
   <numFmts count="1">
     <numFmt numFmtId="45" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <b/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <i/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <b/>
+      <i/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -51,9 +88,12 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1" applyFill="1"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf xfId="0" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf xfId="0" borderId="0" fillId="0" fontId="0" numFmtId="45"/>
+    <xf xfId="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf xfId="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf xfId="0" borderId="0" fillId="0" fontId="3" numFmtId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="normal" builtinId="0"/>
@@ -64,7 +104,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -99,6 +139,26 @@
     <row r="6">
       <c r="A6"/>
     </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8"/>
+    <row r="9">
+      <c r="A9" t="s" s="2">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10"/>
+    <row r="11">
+      <c r="A11" t="s" s="4">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
 </worksheet>
 </file>
</xml_diff>